<commit_message>
Confirms that insats is defined in insatsdef, and first prod run.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -266,13 +266,13 @@
     <t>Insater för kontroll</t>
   </si>
   <si>
-    <t>D:\RPA\RPA_028\Temp</t>
-  </si>
-  <si>
     <t>InsatserNotToHandle</t>
   </si>
   <si>
     <t>InsatserAttInteHantera</t>
+  </si>
+  <si>
+    <t>\\safs008\RPA\VoF\RPA_028\Temp</t>
   </si>
 </sst>
 </file>
@@ -338,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -354,6 +354,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
@@ -671,7 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1858,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1931,8 +1932,8 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>80</v>
+      <c r="B5" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -3015,6 +3016,9 @@
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3129,10 +3133,10 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
         <v>81</v>
-      </c>
-      <c r="B9" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Max 3 Consecutive system exception and removed assign for mailbody from config.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -185,9 +185,6 @@
     <t>MailSubject</t>
   </si>
   <si>
-    <t>MailBody</t>
-  </si>
-  <si>
     <t>MailServerAddress</t>
   </si>
   <si>
@@ -203,9 +200,6 @@
     <t>MailSenderName</t>
   </si>
   <si>
-    <t>No Reply RPA_024</t>
-  </si>
-  <si>
     <t>_KLAR</t>
   </si>
   <si>
@@ -224,9 +218,6 @@
     <t>MailSenderNameorg</t>
   </si>
   <si>
-    <t>TestMailBody</t>
-  </si>
-  <si>
     <t>ExcelFilePrefix</t>
   </si>
   <si>
@@ -248,12 +239,6 @@
     <t>ExcelLösenord</t>
   </si>
   <si>
-    <t>D:\RPA\RPA_028\Output\</t>
-  </si>
-  <si>
-    <t>D:\RPA\RPA_028\Input\</t>
-  </si>
-  <si>
     <t>SheetName</t>
   </si>
   <si>
@@ -273,6 +258,9 @@
   </si>
   <si>
     <t>\\safs008\RPA\VoF\RPA_028\Temp</t>
+  </si>
+  <si>
+    <t>No Reply RPA_028</t>
   </si>
 </sst>
 </file>
@@ -312,7 +300,9 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -349,12 +339,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
@@ -670,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -722,8 +710,8 @@
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>79</v>
+      <c r="B2" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -743,138 +731,117 @@
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>78</v>
+      <c r="B5" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>75</v>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
       </c>
     </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>49</v>
+      <c r="A8" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
+        <v>68</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="B15" s="7">
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>66</v>
+      <c r="A16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>72</v>
+        <v>57</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="8">
-        <v>25</v>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>70</v>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A24" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A27" s="2"/>
+    </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A30" s="2"/>
-    </row>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -1841,14 +1808,11 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B23" r:id="rId1"/>
-    <hyperlink ref="B19" r:id="rId2"/>
+    <hyperlink ref="B20" r:id="rId1"/>
+    <hyperlink ref="B16" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1860,7 +1824,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1921,7 +1885,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>39</v>
@@ -1932,15 +1896,15 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>82</v>
+      <c r="B5" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B6" s="8"/>
+      <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
@@ -3028,7 +2992,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3092,7 +3056,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B4" t="s">
@@ -3109,34 +3073,34 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3146,22 +3110,24 @@
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:1" ht="14.25" customHeight="1">
+      <c r="A30" s="9"/>
+    </row>
+    <row r="31" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Counter for how many rows without any reported hours and Uptade Config (sender mail and subject and name)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -206,18 +206,6 @@
     <t>_HANTERAS</t>
   </si>
   <si>
-    <t>Testsubject</t>
-  </si>
-  <si>
-    <t>MailSenderAddressorg</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>MailSenderNameorg</t>
-  </si>
-  <si>
     <t>ExcelFilePrefix</t>
   </si>
   <si>
@@ -227,9 +215,6 @@
     <t>ExcelSökvägInsatsDefinition</t>
   </si>
   <si>
-    <t>theresia.lundkvist@sundsvall.se</t>
-  </si>
-  <si>
     <t>ExcelPassword</t>
   </si>
   <si>
@@ -260,7 +245,10 @@
     <t>\\safs008\RPA\VoF\RPA_028\Temp</t>
   </si>
   <si>
-    <t>No Reply RPA_028</t>
+    <t>Ava</t>
+  </si>
+  <si>
+    <t>Månadssummering av hemtjänsttimmar</t>
   </si>
 </sst>
 </file>
@@ -660,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -711,7 +699,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -732,7 +720,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>21</v>
@@ -743,7 +731,7 @@
         <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -766,10 +754,10 @@
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -778,7 +766,7 @@
         <v>52</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -786,7 +774,7 @@
         <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
@@ -802,7 +790,7 @@
         <v>55</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
@@ -810,26 +798,18 @@
         <v>57</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>56</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1811,11 +1791,10 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B20" r:id="rId1"/>
-    <hyperlink ref="B16" r:id="rId2"/>
+    <hyperlink ref="B16" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1823,7 +1802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1897,7 +1876,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -3073,34 +3052,34 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Creates new file and moves original file to new folder.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>Insatser för kontroll</t>
+  </si>
+  <si>
+    <t>OrgFolder</t>
+  </si>
+  <si>
+    <t>TempFileFilePath</t>
   </si>
 </sst>
 </file>
@@ -648,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2970,8 +2976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3082,8 +3088,22 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>